<commit_message>
ADRF-RC manual change in a spreadsheet, not code
</commit_message>
<xml_diff>
--- a/string_matching/ADRF-RC Crosslink/ADRF-RC crosslink.xlsx
+++ b/string_matching/ADRF-RC Crosslink/ADRF-RC crosslink.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ernestogimeno/PycharmProjects/RCGraph/string_matching/ADRF-RC Crosslink/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C65346C-9D8A-E74B-AF9E-13EFC87B0D84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908D0CDB-0C20-7D45-A2C3-B101BB8CBFA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="consolidated_matches" sheetId="1" r:id="rId1"/>
@@ -3285,11 +3285,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:N124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="A1:P124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3962,15 +3963,15 @@
     </row>
     <row r="15" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="b">
-        <f>I15=J15</f>
+        <f t="shared" ref="A15:A46" si="3">I15=J15</f>
         <v>1</v>
       </c>
       <c r="B15" s="1" t="b">
-        <f>K15=L15</f>
+        <f t="shared" ref="B15:B46" si="4">K15=L15</f>
         <v>0</v>
       </c>
       <c r="C15" s="1" t="b">
-        <f>G15=H15</f>
+        <f t="shared" ref="C15:C46" si="5">G15=H15</f>
         <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -4009,15 +4010,15 @@
     </row>
     <row r="16" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="b">
-        <f>I16=J16</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="B16" s="1" t="b">
-        <f>K16=L16</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C16" s="1" t="b">
-        <f>G16=H16</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -4056,15 +4057,15 @@
     </row>
     <row r="17" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="b">
-        <f>I17=J17</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B17" s="1" t="b">
-        <f>K17=L17</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C17" s="1" t="b">
-        <f>G17=H17</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -4103,15 +4104,15 @@
     </row>
     <row r="18" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="b">
-        <f>I18=J18</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B18" s="1" t="b">
-        <f>K18=L18</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C18" s="1" t="b">
-        <f>G18=H18</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -4150,15 +4151,15 @@
     </row>
     <row r="19" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="b">
-        <f>I19=J19</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B19" s="1" t="b">
-        <f>K19=L19</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C19" s="1" t="b">
-        <f>G19=H19</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -4197,15 +4198,15 @@
     </row>
     <row r="20" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="b">
-        <f>I20=J20</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B20" s="1" t="b">
-        <f>K20=L20</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C20" s="1" t="b">
-        <f>G20=H20</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -4244,15 +4245,15 @@
     </row>
     <row r="21" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="b">
-        <f>I21=J21</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B21" s="1" t="b">
-        <f>K21=L21</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C21" s="1" t="b">
-        <f>G21=H21</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -4291,15 +4292,15 @@
     </row>
     <row r="22" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="b">
-        <f>I22=J22</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B22" s="1" t="b">
-        <f>K22=L22</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C22" s="1" t="b">
-        <f>G22=H22</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -4335,15 +4336,15 @@
     </row>
     <row r="23" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="b">
-        <f>I23=J23</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B23" s="1" t="b">
-        <f>K23=L23</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C23" s="1" t="b">
-        <f>G23=H23</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -4382,15 +4383,15 @@
     </row>
     <row r="24" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="b">
-        <f>I24=J24</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B24" s="1" t="b">
-        <f>K24=L24</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C24" s="1" t="b">
-        <f>G24=H24</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -4429,15 +4430,15 @@
     </row>
     <row r="25" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="b">
-        <f>I25=J25</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B25" s="1" t="b">
-        <f>K25=L25</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C25" s="1" t="b">
-        <f>G25=H25</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -4471,17 +4472,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="b">
-        <f>I26=J26</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B26" s="1" t="b">
-        <f>K26=L26</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C26" s="1" t="b">
-        <f>G26=H26</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -4516,17 +4517,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="b">
-        <f>I27=J27</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B27" s="1" t="b">
-        <f>K27=L27</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C27" s="1" t="b">
-        <f>G27=H27</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -4563,17 +4564,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="b">
-        <f>I28=J28</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="B28" s="1" t="b">
-        <f>K28=L28</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C28" s="1" t="b">
-        <f>G28=H28</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -4610,17 +4611,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="b">
-        <f>I29=J29</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="B29" s="1" t="b">
-        <f>K29=L29</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C29" s="1" t="b">
-        <f>G29=H29</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
@@ -4657,17 +4658,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="b">
-        <f>I30=J30</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="B30" s="1" t="b">
-        <f>K30=L30</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C30" s="1" t="b">
-        <f>G30=H30</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D30" s="2" t="s">
@@ -4704,17 +4705,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="b">
-        <f>I31=J31</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="B31" s="1" t="b">
-        <f>K31=L31</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C31" s="1" t="b">
-        <f>G31=H31</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D31" s="2" t="s">
@@ -4751,17 +4752,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="b">
-        <f>I32=J32</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B32" s="1" t="b">
-        <f>K32=L32</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C32" s="1" t="b">
-        <f>G32=H32</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -4798,17 +4799,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="b">
-        <f>I33=J33</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B33" s="1" t="b">
-        <f>K33=L33</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C33" s="1" t="b">
-        <f>G33=H33</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -4845,17 +4846,17 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="b">
-        <f>I34=J34</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B34" s="1" t="b">
-        <f>K34=L34</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C34" s="1" t="b">
-        <f>G34=H34</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -4892,17 +4893,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="b">
-        <f>I35=J35</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B35" s="1" t="b">
-        <f>K35=L35</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C35" s="1" t="b">
-        <f>G35=H35</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -4939,17 +4940,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="b">
-        <f>I36=J36</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B36" s="1" t="b">
-        <f>K36=L36</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C36" s="1" t="b">
-        <f>G36=H36</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -4986,17 +4987,17 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="b">
-        <f>I37=J37</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B37" s="1" t="b">
-        <f>K37=L37</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C37" s="1" t="b">
-        <f>G37=H37</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -5033,17 +5034,17 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="b">
-        <f>I38=J38</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="B38" s="1" t="b">
-        <f>K38=L38</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C38" s="1" t="b">
-        <f>G38=H38</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -5080,17 +5081,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="b">
-        <f>I39=J39</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B39" s="1" t="b">
-        <f>K39=L39</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C39" s="1" t="b">
-        <f>G39=H39</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -5127,17 +5128,17 @@
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="b">
-        <f>I40=J40</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B40" s="1" t="b">
-        <f>K40=L40</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C40" s="1" t="b">
-        <f>G40=H40</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D40" s="2" t="s">
@@ -5174,17 +5175,17 @@
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="b">
-        <f>I41=J41</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B41" s="1" t="b">
-        <f>K41=L41</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C41" s="1" t="b">
-        <f>G41=H41</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -5221,17 +5222,17 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="b">
-        <f>I42=J42</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B42" s="1" t="b">
-        <f>K42=L42</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C42" s="1" t="b">
-        <f>G42=H42</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -5268,17 +5269,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="b">
-        <f>I43=J43</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B43" s="1" t="b">
-        <f>K43=L43</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C43" s="1" t="b">
-        <f>G43=H43</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -5315,17 +5316,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="b">
-        <f>I44=J44</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="B44" s="1" t="b">
-        <f>K44=L44</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C44" s="1" t="b">
-        <f>G44=H44</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -5359,17 +5360,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="b">
-        <f>I45=J45</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B45" s="1" t="b">
-        <f>K45=L45</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C45" s="1" t="b">
-        <f>G45=H45</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -5406,17 +5407,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="b">
-        <f>I46=J46</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="B46" s="1" t="b">
-        <f>K46=L46</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C46" s="1" t="b">
-        <f>G46=H46</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -5450,17 +5451,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="b">
-        <f>I47=J47</f>
+        <f t="shared" ref="A47:A78" si="6">I47=J47</f>
         <v>1</v>
       </c>
       <c r="B47" s="1" t="b">
-        <f>K47=L47</f>
+        <f t="shared" ref="B47:B78" si="7">K47=L47</f>
         <v>0</v>
       </c>
       <c r="C47" s="1" t="b">
-        <f>G47=H47</f>
+        <f t="shared" ref="C47:C78" si="8">G47=H47</f>
         <v>0</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -5494,17 +5495,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="b">
-        <f>I48=J48</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="B48" s="1" t="b">
-        <f>K48=L48</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C48" s="1" t="b">
-        <f>G48=H48</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -5541,17 +5542,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="b">
-        <f>I49=J49</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="B49" s="1" t="b">
-        <f>K49=L49</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C49" s="1" t="b">
-        <f>G49=H49</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -5588,17 +5589,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="b">
-        <f>I50=J50</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="B50" s="1" t="b">
-        <f>K50=L50</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C50" s="1" t="b">
-        <f>G50=H50</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -5635,17 +5636,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="b">
-        <f>I51=J51</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="B51" s="1" t="b">
-        <f>K51=L51</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C51" s="1" t="b">
-        <f>G51=H51</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -5682,17 +5683,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="b">
-        <f>I52=J52</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="B52" s="1" t="b">
-        <f>K52=L52</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C52" s="1" t="b">
-        <f>G52=H52</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -5729,17 +5730,17 @@
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="b">
-        <f>I53=J53</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="B53" s="1" t="b">
-        <f>K53=L53</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C53" s="1" t="b">
-        <f>G53=H53</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -5776,17 +5777,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="b">
-        <f>I54=J54</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B54" s="1" t="b">
-        <f>K54=L54</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C54" s="1" t="b">
-        <f>G54=H54</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -5823,17 +5824,17 @@
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="b">
-        <f>I55=J55</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B55" s="1" t="b">
-        <f>K55=L55</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C55" s="1" t="b">
-        <f>G55=H55</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -5870,17 +5871,17 @@
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="b">
-        <f>I56=J56</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B56" s="1" t="b">
-        <f>K56=L56</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C56" s="1" t="b">
-        <f>G56=H56</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -5914,17 +5915,17 @@
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="b">
-        <f>I57=J57</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B57" s="1" t="b">
-        <f>K57=L57</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C57" s="1" t="b">
-        <f>G57=H57</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -5958,17 +5959,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="b">
-        <f>I58=J58</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B58" s="1" t="b">
-        <f>K58=L58</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C58" s="1" t="b">
-        <f>G58=H58</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -6002,17 +6003,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="b">
-        <f>I59=J59</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B59" s="1" t="b">
-        <f>K59=L59</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C59" s="1" t="b">
-        <f>G59=H59</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D59" s="2" t="s">
@@ -6047,17 +6048,17 @@
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="b">
-        <f>I60=J60</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B60" s="1" t="b">
-        <f>K60=L60</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C60" s="1" t="b">
-        <f>G60=H60</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D60" s="2" t="s">
@@ -6092,17 +6093,17 @@
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="b">
-        <f>I61=J61</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B61" s="1" t="b">
-        <f>K61=L61</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C61" s="1" t="b">
-        <f>G61=H61</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -6139,17 +6140,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="b">
-        <f>I62=J62</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B62" s="1" t="b">
-        <f>K62=L62</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="C62" s="1" t="b">
-        <f>G62=H62</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -6186,17 +6187,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="b">
-        <f>I63=J63</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B63" s="1" t="b">
-        <f>K63=L63</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="C63" s="1" t="b">
-        <f>G63=H63</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -6233,17 +6234,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="b">
-        <f>I64=J64</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B64" s="1" t="b">
-        <f>K64=L64</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="C64" s="1" t="b">
-        <f>G64=H64</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -6280,17 +6281,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="b">
-        <f>I65=J65</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B65" s="1" t="b">
-        <f>K65=L65</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C65" s="1" t="b">
-        <f>G65=H65</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -6327,17 +6328,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="b">
-        <f>I66=J66</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B66" s="1" t="b">
-        <f>K66=L66</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C66" s="1" t="b">
-        <f>G66=H66</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -6374,17 +6375,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="b">
-        <f>I67=J67</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B67" s="1" t="b">
-        <f>K67=L67</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C67" s="1" t="b">
-        <f>G67=H67</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -6421,17 +6422,17 @@
         <v>34</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="b">
-        <f>I68=J68</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B68" s="1" t="b">
-        <f>K68=L68</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C68" s="1" t="b">
-        <f>G68=H68</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -6468,17 +6469,17 @@
         <v>34</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="b">
-        <f>I69=J69</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B69" s="1" t="b">
-        <f>K69=L69</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C69" s="1" t="b">
-        <f>G69=H69</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -6515,17 +6516,17 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="b">
-        <f>I70=J70</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B70" s="1" t="b">
-        <f>K70=L70</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C70" s="1" t="b">
-        <f>G70=H70</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -6562,17 +6563,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="b">
-        <f>I71=J71</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B71" s="1" t="b">
-        <f>K71=L71</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C71" s="1" t="b">
-        <f>G71=H71</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -6609,17 +6610,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="b">
-        <f>I72=J72</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B72" s="1" t="b">
-        <f>K72=L72</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C72" s="1" t="b">
-        <f>G72=H72</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -6656,17 +6657,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="b">
-        <f>I73=J73</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B73" s="1" t="b">
-        <f>K73=L73</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="C73" s="1" t="b">
-        <f>G73=H73</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -6703,17 +6704,17 @@
         <v>33</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="b">
-        <f>I74=J74</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B74" s="1" t="b">
-        <f>K74=L74</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="C74" s="1" t="b">
-        <f>G74=H74</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -6750,17 +6751,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="b">
-        <f>I75=J75</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B75" s="1" t="b">
-        <f>K75=L75</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C75" s="1" t="b">
-        <f>G75=H75</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -6797,17 +6798,17 @@
         <v>19</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="b">
-        <f>I76=J76</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B76" s="1" t="b">
-        <f>K76=L76</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C76" s="1" t="b">
-        <f>G76=H76</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -6844,17 +6845,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="b">
-        <f>I77=J77</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="B77" s="1" t="b">
-        <f>K77=L77</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C77" s="1" t="b">
-        <f>G77=H77</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -6891,17 +6892,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="b">
-        <f>I78=J78</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="B78" s="1" t="b">
-        <f>K78=L78</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C78" s="1" t="b">
-        <f>G78=H78</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -6938,17 +6939,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="b">
-        <f>I79=J79</f>
+        <f t="shared" ref="A79:A110" si="9">I79=J79</f>
         <v>1</v>
       </c>
       <c r="B79" s="1" t="b">
-        <f>K79=L79</f>
+        <f t="shared" ref="B79:B110" si="10">K79=L79</f>
         <v>0</v>
       </c>
       <c r="C79" s="1" t="b">
-        <f>G79=H79</f>
+        <f t="shared" ref="C79:C110" si="11">G79=H79</f>
         <v>0</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -6985,17 +6986,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="b">
-        <f>I80=J80</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B80" s="1" t="b">
-        <f>K80=L80</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C80" s="1" t="b">
-        <f>G80=H80</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -7032,17 +7033,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="b">
-        <f>I81=J81</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="B81" s="1" t="b">
-        <f>K81=L81</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="C81" s="1" t="b">
-        <f>G81=H81</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -7079,17 +7080,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="b">
-        <f>I82=J82</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="B82" s="1" t="b">
-        <f>K82=L82</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="C82" s="1" t="b">
-        <f>G82=H82</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -7126,17 +7127,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="b">
-        <f>I83=J83</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="B83" s="1" t="b">
-        <f>K83=L83</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="C83" s="1" t="b">
-        <f>G83=H83</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -7173,17 +7174,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="b">
-        <f>I84=J84</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="B84" s="1" t="b">
-        <f>K84=L84</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="C84" s="1" t="b">
-        <f>G84=H84</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -7220,17 +7221,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="b">
-        <f>I85=J85</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="B85" s="1" t="b">
-        <f>K85=L85</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="C85" s="1" t="b">
-        <f>G85=H85</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -7267,17 +7268,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="b">
-        <f>I86=J86</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="B86" s="1" t="b">
-        <f>K86=L86</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="C86" s="1" t="b">
-        <f>G86=H86</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D86" s="1" t="s">
@@ -7314,17 +7315,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="b">
-        <f>I87=J87</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="B87" s="1" t="b">
-        <f>K87=L87</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C87" s="1" t="b">
-        <f>G87=H87</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D87" s="1" t="s">
@@ -7361,17 +7362,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="b">
-        <f>I88=J88</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="B88" s="1" t="b">
-        <f>K88=L88</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C88" s="1" t="b">
-        <f>G88=H88</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -7408,17 +7409,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="b">
-        <f>I89=J89</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="B89" s="1" t="b">
-        <f>K89=L89</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C89" s="1" t="b">
-        <f>G89=H89</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -7455,17 +7456,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="b">
-        <f>I90=J90</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="B90" s="1" t="b">
-        <f>K90=L90</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C90" s="1" t="b">
-        <f>G90=H90</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -7502,17 +7503,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="b">
-        <f>I91=J91</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="B91" s="1" t="b">
-        <f>K91=L91</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C91" s="1" t="b">
-        <f>G91=H91</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -7549,17 +7550,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="b">
-        <f>I92=J92</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="B92" s="1" t="b">
-        <f>K92=L92</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C92" s="1" t="b">
-        <f>G92=H92</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -7596,17 +7597,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="b">
-        <f>I93=J93</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="B93" s="1" t="b">
-        <f>K93=L93</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C93" s="1" t="b">
-        <f>G93=H93</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -7643,17 +7644,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="b">
-        <f>I94=J94</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="B94" s="1" t="b">
-        <f>K94=L94</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C94" s="1" t="b">
-        <f>G94=H94</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -7690,17 +7691,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="b">
-        <f>I95=J95</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B95" s="1" t="b">
-        <f>K95=L95</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="C95" s="1" t="b">
-        <f>G95=H95</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -7737,17 +7738,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="b">
-        <f>I96=J96</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B96" s="1" t="b">
-        <f>K96=L96</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="C96" s="1" t="b">
-        <f>G96=H96</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -7784,17 +7785,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="b">
-        <f>I97=J97</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B97" s="1" t="b">
-        <f>K97=L97</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="C97" s="1" t="b">
-        <f>G97=H97</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D97" s="2" t="s">
@@ -7831,17 +7832,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="b">
-        <f>I98=J98</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B98" s="1" t="b">
-        <f>K98=L98</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="C98" s="1" t="b">
-        <f>G98=H98</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -7878,17 +7879,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="b">
-        <f>I99=J99</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B99" s="1" t="b">
-        <f>K99=L99</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="C99" s="1" t="b">
-        <f>G99=H99</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -7925,17 +7926,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="b">
-        <f>I100=J100</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="B100" s="1" t="b">
-        <f>K100=L100</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C100" s="1" t="b">
-        <f>G100=H100</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -7972,17 +7973,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="b">
-        <f>I101=J101</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B101" s="1" t="b">
-        <f>K101=L101</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C101" s="1" t="b">
-        <f>G101=H101</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -8019,17 +8020,17 @@
         <v>46</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="b">
-        <f>I102=J102</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="B102" s="1" t="b">
-        <f>K102=L102</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C102" s="1" t="b">
-        <f>G102=H102</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -8066,17 +8067,17 @@
         <v>31</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="b">
-        <f>I103=J103</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="B103" s="1" t="b">
-        <f>K103=L103</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C103" s="1" t="b">
-        <f>G103=H103</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D103" s="1" t="s">
@@ -8113,17 +8114,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="b">
-        <f>I104=J104</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B104" s="1" t="b">
-        <f>K104=L104</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="C104" s="1" t="b">
-        <f>G104=H104</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -8160,17 +8161,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="b">
-        <f>I105=J105</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B105" s="1" t="b">
-        <f>K105=L105</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C105" s="1" t="b">
-        <f>G105=H105</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -8207,17 +8208,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="b">
-        <f>I106=J106</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B106" s="1" t="b">
-        <f>K106=L106</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C106" s="1" t="b">
-        <f>G106=H106</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D106" s="1" t="s">
@@ -8254,17 +8255,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="b">
-        <f>I107=J107</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B107" s="1" t="b">
-        <f>K107=L107</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C107" s="1" t="b">
-        <f>G107=H107</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -8301,17 +8302,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="b">
-        <f>I108=J108</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B108" s="1" t="b">
-        <f>K108=L108</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C108" s="1" t="b">
-        <f>G108=H108</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D108" s="1" t="s">
@@ -8348,17 +8349,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="b">
-        <f>I109=J109</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B109" s="1" t="b">
-        <f>K109=L109</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C109" s="1" t="b">
-        <f>G109=H109</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D109" s="1" t="s">
@@ -8395,17 +8396,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="b">
-        <f>I110=J110</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B110" s="1" t="b">
-        <f>K110=L110</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="C110" s="1" t="b">
-        <f>G110=H110</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D110" s="1" t="s">
@@ -8442,17 +8443,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="b">
-        <f>I111=J111</f>
+        <f t="shared" ref="A111:A124" si="12">I111=J111</f>
         <v>0</v>
       </c>
       <c r="B111" s="1" t="b">
-        <f>K111=L111</f>
+        <f t="shared" ref="B111:B124" si="13">K111=L111</f>
         <v>0</v>
       </c>
       <c r="C111" s="1" t="b">
-        <f>G111=H111</f>
+        <f t="shared" ref="C111:C124" si="14">G111=H111</f>
         <v>0</v>
       </c>
       <c r="D111" s="1" t="s">
@@ -8486,17 +8487,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="b">
-        <f>I112=J112</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="B112" s="1" t="b">
-        <f>K112=L112</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="C112" s="1" t="b">
-        <f>G112=H112</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="D112" s="1" t="s">
@@ -8533,17 +8534,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="b">
-        <f>I113=J113</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="B113" s="1" t="b">
-        <f>K113=L113</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="C113" s="1" t="b">
-        <f>G113=H113</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="D113" s="1" t="s">
@@ -8580,17 +8581,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="b">
-        <f>I114=J114</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="B114" s="1" t="b">
-        <f>K114=L114</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="C114" s="1" t="b">
-        <f>G114=H114</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="D114" s="1" t="s">
@@ -8627,17 +8628,17 @@
         <v>47</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="b">
-        <f>I115=J115</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="B115" s="1" t="b">
-        <f>K115=L115</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="C115" s="1" t="b">
-        <f>G115=H115</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="D115" s="2" t="s">
@@ -8674,17 +8675,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="116" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="b">
-        <f>I116=J116</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="B116" s="1" t="b">
-        <f>K116=L116</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="C116" s="1" t="b">
-        <f>G116=H116</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="D116" s="1" t="s">
@@ -8721,17 +8722,17 @@
         <v>49</v>
       </c>
     </row>
-    <row r="117" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="b">
-        <f>I117=J117</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="B117" s="1" t="b">
-        <f>K117=L117</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="C117" s="1" t="b">
-        <f>G117=H117</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="D117" s="1" t="s">
@@ -8765,17 +8766,17 @@
         <v>37</v>
       </c>
     </row>
-    <row r="118" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="b">
-        <f>I118=J118</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="B118" s="1" t="b">
-        <f>K118=L118</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="C118" s="1" t="b">
-        <f>G118=H118</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="D118" s="1" t="s">
@@ -8812,17 +8813,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="b">
-        <f>I119=J119</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="B119" s="1" t="b">
-        <f>K119=L119</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="C119" s="1" t="b">
-        <f>G119=H119</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="D119" s="1" t="s">
@@ -8859,17 +8860,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="b">
-        <f>I120=J120</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="B120" s="1" t="b">
-        <f>K120=L120</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="C120" s="1" t="b">
-        <f>G120=H120</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="D120" s="2" t="s">
@@ -8906,17 +8907,17 @@
         <v>54</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="b">
-        <f>I121=J121</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="B121" s="1" t="b">
-        <f>K121=L121</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="C121" s="1" t="b">
-        <f>G121=H121</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="D121" s="2" t="s">
@@ -8953,17 +8954,17 @@
         <v>54</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="b">
-        <f>I122=J122</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="B122" s="1" t="b">
-        <f>K122=L122</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="C122" s="1" t="b">
-        <f>G122=H122</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="D122" s="1" t="s">
@@ -9000,17 +9001,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="b">
-        <f>I123=J123</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="B123" s="1" t="b">
-        <f>K123=L123</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="C123" s="1" t="b">
-        <f>G123=H123</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="D123" s="1" t="s">
@@ -9047,17 +9048,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:14" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="b">
-        <f>I124=J124</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="B124" s="1" t="b">
-        <f>K124=L124</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="C124" s="1" t="b">
-        <f>G124=H124</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="D124" s="1" t="s">
@@ -9096,6 +9097,15 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:N124" xr:uid="{9E679407-7E0D-0B44-BA23-8B3CD292B21B}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="maybe not. Is open data version comparable to not public version?"/>
+        <filter val="maybe yes"/>
+        <filter val="maybe yes, but looks like &quot;siblings&quot; datasets"/>
+        <filter val="no"/>
+        <filter val="probably not"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N124">
       <sortCondition ref="D2:D124"/>
       <sortCondition ref="E2:E124"/>
@@ -9116,8 +9126,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G136"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9230,7 +9240,7 @@
         <v>adrf-000085</v>
       </c>
     </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>32</v>
       </c>
@@ -9251,7 +9261,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>39</v>
       </c>
@@ -9272,7 +9282,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>41</v>
       </c>
@@ -10472,7 +10482,7 @@
         <v>adrf-000038</v>
       </c>
     </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>177</v>
       </c>
@@ -10493,7 +10503,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>181</v>
       </c>
@@ -10514,7 +10524,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>183</v>
       </c>
@@ -10535,7 +10545,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>185</v>
       </c>
@@ -10556,7 +10566,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>187</v>
       </c>
@@ -10787,7 +10797,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>264</v>
       </c>
@@ -10850,7 +10860,7 @@
         <v>adrf-000056</v>
       </c>
     </row>
-    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>277</v>
       </c>
@@ -10871,7 +10881,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>564</v>
       </c>
@@ -10892,7 +10902,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>566</v>
       </c>
@@ -11024,7 +11034,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>576</v>
       </c>
@@ -11045,7 +11055,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>677</v>
       </c>
@@ -11069,7 +11079,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>582</v>
       </c>
@@ -11090,7 +11100,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>584</v>
       </c>
@@ -11159,7 +11169,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
         <v>103</v>
       </c>
@@ -11180,7 +11190,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
         <v>300</v>
       </c>
@@ -11201,7 +11211,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
         <v>307</v>
       </c>
@@ -11270,7 +11280,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>315</v>
       </c>
@@ -11360,7 +11370,7 @@
         <v>adrf-000097</v>
       </c>
     </row>
-    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>325</v>
       </c>
@@ -11381,7 +11391,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
         <v>332</v>
       </c>
@@ -11492,7 +11502,7 @@
         <v>adrf-000137</v>
       </c>
     </row>
-    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
         <v>237</v>
       </c>
@@ -11651,7 +11661,7 @@
         <v>adrf-000120</v>
       </c>
     </row>
-    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
         <v>627</v>
       </c>
@@ -11906,7 +11916,7 @@
         <v>adrf-000130</v>
       </c>
     </row>
-    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
         <v>353</v>
       </c>
@@ -11927,7 +11937,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
         <v>375</v>
       </c>
@@ -11948,7 +11958,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
         <v>394</v>
       </c>
@@ -12011,7 +12021,7 @@
         <v>adrf-000144</v>
       </c>
     </row>
-    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>723</v>
       </c>
@@ -12059,7 +12069,7 @@
         <v>adrf-000146</v>
       </c>
     </row>
-    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>725</v>
       </c>
@@ -12083,7 +12093,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
         <v>726</v>
       </c>
@@ -12109,11 +12119,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:G136" xr:uid="{9BD15B37-F690-3F4B-A82B-53B82DBC75CA}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Unknown"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="6">
       <filters>
         <filter val="#N/A"/>
@@ -12129,7 +12134,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12787,7 +12792,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13182,8 +13187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF799CE-C596-6143-AA85-90FFEC36991E}">
   <dimension ref="A1:L92"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16845,7 +16850,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>